<commit_message>
highlighted bad samples in sequence file
</commit_message>
<xml_diff>
--- a/analyses/DNR_SRM_20170902/2017-07-28-SRM-Sequence-File.xlsx
+++ b/analyses/DNR_SRM_20170902/2017-07-28-SRM-Sequence-File.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-oa/analyses/DNR_SRM_20170902/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="355">
   <si>
     <t>File Name</t>
   </si>
@@ -1084,6 +1084,15 @@
   </si>
   <si>
     <t>Time injected</t>
+  </si>
+  <si>
+    <t>O49-1</t>
+  </si>
+  <si>
+    <t>O52-1</t>
+  </si>
+  <si>
+    <t>O102-1</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1912,7 @@
   <dimension ref="A1:I190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2070,7 +2079,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>352</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -2093,7 +2102,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>353</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -2116,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>354</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
marked bivalve_16 as no data
</commit_message>
<xml_diff>
--- a/analyses/DNR_SRM_20170902/2017-07-28-SRM-Sequence-File.xlsx
+++ b/analyses/DNR_SRM_20170902/2017-07-28-SRM-Sequence-File.xlsx
@@ -1099,7 +1099,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1230,6 +1230,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1576,7 +1583,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1586,6 +1593,10 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1912,7 +1923,7 @@
   <dimension ref="A1:I190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2439,26 +2450,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="6">
         <v>16</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="D23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="5">
         <v>2</v>
       </c>
     </row>

</xml_diff>